<commit_message>
added filter on each sheet  and generated summary sheet from combined sheet
</commit_message>
<xml_diff>
--- a/output/team_summary.xlsx
+++ b/output/team_summary.xlsx
@@ -11,33 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>BSO Associate Name</t>
-  </si>
-  <si>
-    <t>No Action</t>
-  </si>
-  <si>
-    <t>billed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billed </t>
-  </si>
-  <si>
-    <t>billled</t>
-  </si>
-  <si>
-    <t>no action</t>
   </si>
   <si>
     <t>Grand Total</t>
   </si>
   <si>
-    <t>dinesh kumar</t>
+    <t>Emily Harris</t>
   </si>
   <si>
-    <t>Nitish kumar</t>
+    <t>John Hill</t>
+  </si>
+  <si>
+    <t>Sophia Carter</t>
   </si>
 </sst>
 </file>
@@ -433,13 +421,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:AB5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="16" width="15" customWidth="1"/>
+    <col min="1" max="28" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,184 +435,426 @@
         <v>1054</v>
       </c>
       <c r="C1" s="1">
+        <v>1059</v>
+      </c>
+      <c r="D1" s="1">
         <v>1216</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>1225</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
+        <v>12773</v>
+      </c>
+      <c r="G1" s="1">
         <v>12774</v>
       </c>
-      <c r="F1" s="1">
+      <c r="H1" s="1">
+        <v>12873</v>
+      </c>
+      <c r="I1" s="1">
+        <v>12888</v>
+      </c>
+      <c r="J1" s="1">
+        <v>12889</v>
+      </c>
+      <c r="K1" s="1">
+        <v>12901</v>
+      </c>
+      <c r="L1" s="1">
         <v>12906</v>
       </c>
-      <c r="G1" s="1">
+      <c r="M1" s="1">
+        <v>12968</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12969</v>
+      </c>
+      <c r="O1" s="1">
         <v>13017</v>
       </c>
-      <c r="H1" s="1">
+      <c r="P1" s="1">
         <v>13018</v>
       </c>
-      <c r="I1" s="1">
+      <c r="Q1" s="1">
+        <v>13140</v>
+      </c>
+      <c r="R1" s="1">
+        <v>14717</v>
+      </c>
+      <c r="S1" s="1">
+        <v>4249</v>
+      </c>
+      <c r="T1" s="1">
+        <v>5711</v>
+      </c>
+      <c r="U1" s="1">
+        <v>5713</v>
+      </c>
+      <c r="V1" s="1">
+        <v>5715</v>
+      </c>
+      <c r="W1" s="1">
+        <v>6264</v>
+      </c>
+      <c r="X1" s="1">
+        <v>6453</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>6464</v>
+      </c>
+      <c r="Z1" s="1">
         <v>6510</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="AA1" s="1">
+        <v>9265</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3</v>
+      </c>
+      <c r="O5" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>64</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="P5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>3</v>
+      </c>
+      <c r="R5" s="2">
+        <v>3</v>
+      </c>
+      <c r="S5" s="2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
+      <c r="T5" s="2">
+        <v>3</v>
+      </c>
+      <c r="U5" s="2">
+        <v>3</v>
+      </c>
+      <c r="V5" s="2">
+        <v>5</v>
+      </c>
+      <c r="W5" s="2">
+        <v>2</v>
+      </c>
+      <c r="X5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="2">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="AA5" s="2">
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>11</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>9</v>
-      </c>
-      <c r="P2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>38</v>
-      </c>
-      <c r="C3">
-        <v>67</v>
-      </c>
-      <c r="D3">
-        <v>43</v>
-      </c>
-      <c r="E3">
-        <v>114</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>42</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>9</v>
-      </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>24</v>
-      </c>
-      <c r="P3">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <v>51</v>
-      </c>
-      <c r="C4" s="2">
-        <v>131</v>
-      </c>
-      <c r="D4" s="2">
-        <v>51</v>
-      </c>
-      <c r="E4" s="2">
-        <v>116</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2">
-        <v>46</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2">
-        <v>20</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>33</v>
-      </c>
-      <c r="P4" s="2">
-        <v>506</v>
+      <c r="AB5" s="2">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>